<commit_message>
Forecast prez + pleb
</commit_message>
<xml_diff>
--- a/files/polls/CHL_2020-1.xlsx
+++ b/files/polls/CHL_2020-1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t>Fecha</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>01/08/2020</t>
+  </si>
+  <si>
+    <t>15/08/2020</t>
   </si>
   <si>
     <t>Encuesta</t>
@@ -217,7 +220,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E45"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -225,16 +228,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -242,7 +245,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1">
         <v>704</v>
@@ -259,7 +262,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>2000</v>
@@ -276,7 +279,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <v>706</v>
@@ -293,7 +296,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>1159</v>
@@ -310,7 +313,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1">
         <v>1014</v>
@@ -327,7 +330,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1">
         <v>1215</v>
@@ -344,7 +347,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1">
         <v>1030</v>
@@ -358,390 +361,390 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="1">
-        <v>562</v>
+        <v>709</v>
       </c>
       <c r="D9" s="1">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1">
-        <v>709</v>
+        <v>1496</v>
       </c>
       <c r="D10" s="1">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E10" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1">
-        <v>1496</v>
+        <v>707</v>
       </c>
       <c r="D11" s="1">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E11" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1">
-        <v>707</v>
+        <v>1000</v>
       </c>
       <c r="D12" s="1">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E12" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1">
-        <v>780</v>
+        <v>950</v>
       </c>
       <c r="D13" s="1">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E13" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1">
-        <v>1000</v>
+        <v>1033</v>
       </c>
       <c r="D14" s="1">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E14" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="1">
-        <v>950</v>
+        <v>709</v>
       </c>
       <c r="D15" s="1">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1">
-        <v>487</v>
+        <v>806</v>
       </c>
       <c r="D16" s="1">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1">
-        <v>1033</v>
+        <v>975</v>
       </c>
       <c r="D17" s="1">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D18" s="1">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1">
-        <v>806</v>
+        <v>709</v>
       </c>
       <c r="D19" s="1">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1">
-        <v>975</v>
+        <v>1045</v>
       </c>
       <c r="D20" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E20" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="1">
-        <v>477</v>
+        <v>705</v>
       </c>
       <c r="D21" s="1">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E21" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
-        <v>708</v>
+        <v>1445</v>
       </c>
       <c r="D22" s="1">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E22" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D23" s="1">
         <v>67</v>
       </c>
       <c r="E23" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D24" s="1">
         <v>70</v>
       </c>
       <c r="E24" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="1">
-        <v>525</v>
+        <v>702</v>
       </c>
       <c r="D25" s="1">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E25" s="1">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1">
-        <v>705</v>
+        <v>796</v>
       </c>
       <c r="D26" s="1">
         <v>67</v>
       </c>
       <c r="E26" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1">
-        <v>1445</v>
+        <v>707</v>
       </c>
       <c r="D27" s="1">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1">
-        <v>705</v>
+        <v>1135</v>
       </c>
       <c r="D28" s="1">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="1">
-        <v>1043</v>
+        <v>702</v>
       </c>
       <c r="D29" s="1">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E29" s="1">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1">
-        <v>583</v>
+        <v>1273</v>
       </c>
       <c r="D30" s="1">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E30" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1">
         <v>702</v>
       </c>
       <c r="D31" s="1">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1">
         <v>25</v>
@@ -749,495 +752,240 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="1">
-        <v>796</v>
+        <v>1230</v>
       </c>
       <c r="D32" s="1">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E32" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C33" s="1">
-        <v>707</v>
+        <v>1270</v>
       </c>
       <c r="D33" s="1">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E33" s="1">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1">
-        <v>1135</v>
+        <v>1227</v>
       </c>
       <c r="D34" s="1">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E34" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="1">
-        <v>690</v>
+        <v>712</v>
       </c>
       <c r="D35" s="1">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E35" s="1">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1">
-        <v>702</v>
+        <v>1209</v>
       </c>
       <c r="D36" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E36" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1">
-        <v>1273</v>
+        <v>1215</v>
       </c>
       <c r="D37" s="1">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E37" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1">
-        <v>702</v>
+        <v>800</v>
       </c>
       <c r="D38" s="1">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E38" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C39" s="1">
-        <v>1230</v>
+        <v>1730</v>
       </c>
       <c r="D39" s="1">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E39" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1">
-        <v>690</v>
+        <v>1260</v>
       </c>
       <c r="D40" s="1">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E40" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1">
-        <v>1270</v>
+        <v>800</v>
       </c>
       <c r="D41" s="1">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E41" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C42" s="1">
-        <v>725</v>
+        <v>1340</v>
       </c>
       <c r="D42" s="1">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E42" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43" s="1">
-        <v>1227</v>
+        <v>800</v>
       </c>
       <c r="D43" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E43" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C44" s="1">
-        <v>736</v>
+        <v>1430</v>
       </c>
       <c r="D44" s="1">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E44" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C45" s="1">
-        <v>712</v>
+        <v>1434</v>
       </c>
       <c r="D45" s="1">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E45" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1209</v>
-      </c>
-      <c r="D46" s="1">
-        <v>70</v>
-      </c>
-      <c r="E46" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="1">
-        <v>724</v>
-      </c>
-      <c r="D47" s="1">
-        <v>85</v>
-      </c>
-      <c r="E47" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1215</v>
-      </c>
-      <c r="D48" s="1">
-        <v>70</v>
-      </c>
-      <c r="E48" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="1">
-        <v>661</v>
-      </c>
-      <c r="D49" s="1">
-        <v>84</v>
-      </c>
-      <c r="E49" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="1">
-        <v>800</v>
-      </c>
-      <c r="D50" s="1">
-        <v>72</v>
-      </c>
-      <c r="E50" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1730</v>
-      </c>
-      <c r="D51" s="1">
-        <v>73</v>
-      </c>
-      <c r="E51" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="1">
-        <v>960</v>
-      </c>
-      <c r="D52" s="1">
-        <v>91</v>
-      </c>
-      <c r="E52" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1260</v>
-      </c>
-      <c r="D53" s="1">
-        <v>68</v>
-      </c>
-      <c r="E53" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="1">
-        <v>670</v>
-      </c>
-      <c r="D54" s="1">
-        <v>90</v>
-      </c>
-      <c r="E54" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>38</v>
-      </c>
-      <c r="B55" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="1">
-        <v>800</v>
-      </c>
-      <c r="D55" s="1">
-        <v>76</v>
-      </c>
-      <c r="E55" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1340</v>
-      </c>
-      <c r="D56" s="1">
-        <v>72</v>
-      </c>
-      <c r="E56" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="1">
-        <v>747</v>
-      </c>
-      <c r="D57" s="1">
-        <v>88</v>
-      </c>
-      <c r="E57" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="1">
-        <v>800</v>
-      </c>
-      <c r="D58" s="1">
-        <v>75</v>
-      </c>
-      <c r="E58" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1430</v>
-      </c>
-      <c r="D59" s="1">
-        <v>77</v>
-      </c>
-      <c r="E59" s="1">
         <v>10</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>41</v>
-      </c>
-      <c r="B60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="1">
-        <v>797</v>
-      </c>
-      <c r="D60" s="1">
-        <v>91</v>
-      </c>
-      <c r="E60" s="1">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data 1 2 3
</commit_message>
<xml_diff>
--- a/files/polls/CHL_2020-1.xlsx
+++ b/files/polls/CHL_2020-1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="56">
   <si>
     <t>Fecha</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>15/08/2020</t>
+  </si>
+  <si>
+    <t>24/08/2020</t>
   </si>
   <si>
     <t>Encuesta</t>
@@ -223,7 +226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F63"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -231,19 +234,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -251,7 +254,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1">
         <v>704</v>
@@ -271,7 +274,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>2000</v>
@@ -291,7 +294,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <v>706</v>
@@ -311,7 +314,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1">
         <v>1159</v>
@@ -331,7 +334,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1">
         <v>1014</v>
@@ -351,7 +354,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1">
         <v>1215</v>
@@ -371,7 +374,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1">
         <v>1030</v>
@@ -388,293 +391,293 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1">
-        <v>709</v>
+        <v>562</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F9" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
-        <v>1496</v>
+        <v>709</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F10" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1">
-        <v>707</v>
+        <v>1496</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
-        <v>1000</v>
+        <v>707</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1">
-        <v>950</v>
+        <v>780</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F13" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
       <c r="C14" s="1">
-        <v>1033</v>
+        <v>1000</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1">
-        <v>709</v>
+        <v>950</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F15" s="1">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="1">
-        <v>806</v>
+        <v>487</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="F16" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1">
-        <v>975</v>
+        <v>1033</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F18" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1">
-        <v>709</v>
+        <v>806</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1">
-        <v>1045</v>
+        <v>975</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1">
-        <v>705</v>
+        <v>477</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="F21" s="1">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1">
-        <v>1445</v>
+        <v>708</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F22" s="1">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1">
-        <v>705</v>
+        <v>709</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -683,18 +686,18 @@
         <v>67</v>
       </c>
       <c r="F23" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -703,38 +706,38 @@
         <v>70</v>
       </c>
       <c r="F24" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1">
-        <v>702</v>
+        <v>525</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="F25" s="1">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1">
-        <v>796</v>
+        <v>705</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -743,95 +746,95 @@
         <v>67</v>
       </c>
       <c r="F26" s="1">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1">
-        <v>707</v>
+        <v>1445</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F27" s="1">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1">
-        <v>1135</v>
+        <v>705</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F28" s="1">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1">
-        <v>702</v>
+        <v>1043</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F29" s="1">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1">
-        <v>1273</v>
+        <v>583</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F30" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="1">
         <v>702</v>
@@ -840,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F31" s="1">
         <v>25</v>
@@ -848,282 +851,642 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1">
-        <v>1230</v>
+        <v>796</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F32" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="1">
-        <v>1270</v>
+        <v>707</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F33" s="1">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1">
-        <v>1227</v>
+        <v>1135</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F34" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1">
-        <v>712</v>
+        <v>690</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F35" s="1">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="1">
-        <v>1209</v>
+        <v>702</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F36" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C37" s="1">
-        <v>1215</v>
+        <v>1273</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F37" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1">
-        <v>800</v>
+        <v>702</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F38" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C39" s="1">
-        <v>1730</v>
+        <v>1230</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F39" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C40" s="1">
-        <v>1260</v>
+        <v>690</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="F40" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="1">
-        <v>800</v>
+        <v>1270</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F41" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1">
-        <v>1340</v>
+        <v>725</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="1">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="F42" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="1">
-        <v>800</v>
+        <v>1227</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F43" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C44" s="1">
-        <v>1430</v>
+        <v>736</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F44" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="1">
+        <v>712</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>65</v>
+      </c>
+      <c r="F45" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1209</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>70</v>
+      </c>
+      <c r="F46" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="1">
+        <v>724</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>85</v>
+      </c>
+      <c r="F47" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1215</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>70</v>
+      </c>
+      <c r="F48" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="1">
+        <v>661</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>84</v>
+      </c>
+      <c r="F49" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1">
+        <v>800</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>72</v>
+      </c>
+      <c r="F50" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1730</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>73</v>
+      </c>
+      <c r="F51" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="1">
+        <v>960</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>91</v>
+      </c>
+      <c r="F52" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1260</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>68</v>
+      </c>
+      <c r="F53" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="1">
+        <v>670</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>90</v>
+      </c>
+      <c r="F54" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="1">
+        <v>800</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>76</v>
+      </c>
+      <c r="F55" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1340</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>72</v>
+      </c>
+      <c r="F56" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="1">
+        <v>747</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1">
+        <v>88</v>
+      </c>
+      <c r="F57" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="1">
+        <v>800</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>75</v>
+      </c>
+      <c r="F58" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1430</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>77</v>
+      </c>
+      <c r="F59" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="1">
+        <v>797</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1">
+        <v>91</v>
+      </c>
+      <c r="F60" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="1">
         <v>1434</v>
       </c>
-      <c r="D45" s="1">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
         <v>68</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F61" s="1">
         <v>10</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1434</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>89</v>
+      </c>
+      <c r="F62" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1940</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>73</v>
+      </c>
+      <c r="F63" s="1">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>